<commit_message>
Added base software files.
</commit_message>
<xml_diff>
--- a/Files/Bunkers.xlsx
+++ b/Files/Bunkers.xlsx
@@ -442,7 +442,7 @@
   <dimension ref="A1:ES77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AI43" sqref="AI43"/>
+      <selection activeCell="DV42" sqref="DV42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3921,10 +3921,10 @@
       <c r="CE17" s="5">
         <v>1</v>
       </c>
-      <c r="CF17" s="6">
-        <v>1</v>
-      </c>
-      <c r="CG17" s="4">
+      <c r="CF17" s="5">
+        <v>1</v>
+      </c>
+      <c r="CG17" s="5">
         <v>1</v>
       </c>
       <c r="CH17" s="5">
@@ -4253,10 +4253,10 @@
       <c r="CE18" s="2">
         <v>1</v>
       </c>
-      <c r="CF18" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG18" s="7">
+      <c r="CF18" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG18" s="2">
         <v>1</v>
       </c>
       <c r="CH18" s="2">
@@ -4475,10 +4475,10 @@
       <c r="CE19" s="2">
         <v>1</v>
       </c>
-      <c r="CF19" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG19" s="7">
+      <c r="CF19" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG19" s="2">
         <v>1</v>
       </c>
       <c r="CH19" s="2">
@@ -4697,10 +4697,10 @@
       <c r="CE20" s="2">
         <v>1</v>
       </c>
-      <c r="CF20" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG20" s="7">
+      <c r="CF20" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG20" s="2">
         <v>1</v>
       </c>
       <c r="CH20" s="2">
@@ -4847,10 +4847,10 @@
       <c r="CE21" s="2">
         <v>1</v>
       </c>
-      <c r="CF21" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG21" s="7">
+      <c r="CF21" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG21" s="2">
         <v>1</v>
       </c>
       <c r="CH21" s="2">
@@ -4982,22 +4982,22 @@
       </c>
     </row>
     <row r="22" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="X22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y22" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="2">
+      <c r="X22" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="5">
         <v>0</v>
       </c>
       <c r="AD22" s="4">
@@ -5015,10 +5015,10 @@
       <c r="AH22" s="5">
         <v>1</v>
       </c>
-      <c r="AI22" s="5">
-        <v>1</v>
-      </c>
-      <c r="AJ22" s="5">
+      <c r="AI22" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ22" s="4">
         <v>1</v>
       </c>
       <c r="AK22" s="5">
@@ -5051,10 +5051,10 @@
       <c r="AT22" s="5">
         <v>1</v>
       </c>
-      <c r="AU22" s="5">
-        <v>1</v>
-      </c>
-      <c r="AV22" s="5">
+      <c r="AU22" s="6">
+        <v>1</v>
+      </c>
+      <c r="AV22" s="4">
         <v>1</v>
       </c>
       <c r="AW22" s="5">
@@ -5087,10 +5087,10 @@
       <c r="BF22" s="5">
         <v>1</v>
       </c>
-      <c r="BG22" s="5">
-        <v>1</v>
-      </c>
-      <c r="BH22" s="5">
+      <c r="BG22" s="6">
+        <v>1</v>
+      </c>
+      <c r="BH22" s="4">
         <v>1</v>
       </c>
       <c r="BI22" s="5">
@@ -5108,58 +5108,58 @@
       <c r="BM22" s="6">
         <v>1</v>
       </c>
-      <c r="BN22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BO22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BP22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BQ22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BR22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BS22" s="2">
-        <v>0</v>
-      </c>
-      <c r="CA22" s="8">
-        <v>1</v>
-      </c>
-      <c r="CB22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CC22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CD22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CE22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CF22" s="10">
-        <v>1</v>
-      </c>
-      <c r="CG22" s="8">
-        <v>1</v>
-      </c>
-      <c r="CH22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CI22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CJ22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CK22" s="9">
-        <v>1</v>
-      </c>
-      <c r="CL22" s="10">
+      <c r="BN22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BO22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BP22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BQ22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BR22" s="5">
+        <v>0</v>
+      </c>
+      <c r="BS22" s="6">
+        <v>0</v>
+      </c>
+      <c r="CA22" s="7">
+        <v>1</v>
+      </c>
+      <c r="CB22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CC22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CD22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CE22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CF22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CH22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CI22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CJ22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CK22" s="2">
+        <v>1</v>
+      </c>
+      <c r="CL22" s="1">
         <v>1</v>
       </c>
       <c r="CR22" s="7">
@@ -5276,7 +5276,7 @@
       </c>
     </row>
     <row r="23" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="X23" s="2">
+      <c r="X23" s="7">
         <v>0</v>
       </c>
       <c r="Y23" s="2">
@@ -5309,10 +5309,10 @@
       <c r="AH23" s="2">
         <v>1</v>
       </c>
-      <c r="AI23" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ23" s="2">
+      <c r="AI23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ23" s="7">
         <v>1</v>
       </c>
       <c r="AK23" s="2">
@@ -5345,10 +5345,10 @@
       <c r="AT23" s="2">
         <v>1</v>
       </c>
-      <c r="AU23" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV23" s="2">
+      <c r="AU23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV23" s="7">
         <v>1</v>
       </c>
       <c r="AW23" s="2">
@@ -5381,10 +5381,10 @@
       <c r="BF23" s="2">
         <v>1</v>
       </c>
-      <c r="BG23" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH23" s="2">
+      <c r="BG23" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH23" s="7">
         <v>1</v>
       </c>
       <c r="BI23" s="2">
@@ -5417,43 +5417,43 @@
       <c r="BR23" s="2">
         <v>0</v>
       </c>
-      <c r="BS23" s="2">
-        <v>0</v>
-      </c>
-      <c r="CA23" s="4">
-        <v>1</v>
-      </c>
-      <c r="CB23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CC23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CD23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CE23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CF23" s="6">
-        <v>1</v>
-      </c>
-      <c r="CG23" s="4">
-        <v>1</v>
-      </c>
-      <c r="CH23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CI23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CJ23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CK23" s="5">
-        <v>1</v>
-      </c>
-      <c r="CL23" s="6">
+      <c r="BS23" s="1">
+        <v>0</v>
+      </c>
+      <c r="CA23" s="7">
+        <v>1</v>
+      </c>
+      <c r="CB23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CC23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CD23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CE23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CF23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CH23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CI23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CJ23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CK23" s="2">
+        <v>1</v>
+      </c>
+      <c r="CL23" s="1">
         <v>1</v>
       </c>
       <c r="CR23" s="7">
@@ -5570,7 +5570,7 @@
       </c>
     </row>
     <row r="24" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="X24" s="2">
+      <c r="X24" s="7">
         <v>0</v>
       </c>
       <c r="Y24" s="2">
@@ -5603,10 +5603,10 @@
       <c r="AH24" s="2">
         <v>1</v>
       </c>
-      <c r="AI24" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ24" s="2">
+      <c r="AI24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="7">
         <v>1</v>
       </c>
       <c r="AK24" s="2">
@@ -5639,10 +5639,10 @@
       <c r="AT24" s="2">
         <v>1</v>
       </c>
-      <c r="AU24" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV24" s="2">
+      <c r="AU24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV24" s="7">
         <v>1</v>
       </c>
       <c r="AW24" s="2">
@@ -5675,10 +5675,10 @@
       <c r="BF24" s="2">
         <v>1</v>
       </c>
-      <c r="BG24" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH24" s="2">
+      <c r="BG24" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH24" s="7">
         <v>1</v>
       </c>
       <c r="BI24" s="2">
@@ -5711,7 +5711,7 @@
       <c r="BR24" s="2">
         <v>0</v>
       </c>
-      <c r="BS24" s="2">
+      <c r="BS24" s="1">
         <v>0</v>
       </c>
       <c r="BT24" s="2"/>
@@ -5736,10 +5736,10 @@
       <c r="CE24" s="2">
         <v>1</v>
       </c>
-      <c r="CF24" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG24" s="7">
+      <c r="CF24" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG24" s="2">
         <v>1</v>
       </c>
       <c r="CH24" s="2">
@@ -5871,7 +5871,7 @@
       </c>
     </row>
     <row r="25" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="X25" s="2">
+      <c r="X25" s="7">
         <v>0</v>
       </c>
       <c r="Y25" s="2">
@@ -5904,10 +5904,10 @@
       <c r="AH25" s="2">
         <v>1</v>
       </c>
-      <c r="AI25" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ25" s="2">
+      <c r="AI25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="7">
         <v>1</v>
       </c>
       <c r="AK25" s="2">
@@ -5940,10 +5940,10 @@
       <c r="AT25" s="2">
         <v>1</v>
       </c>
-      <c r="AU25" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV25" s="2">
+      <c r="AU25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV25" s="7">
         <v>1</v>
       </c>
       <c r="AW25" s="2">
@@ -5976,10 +5976,10 @@
       <c r="BF25" s="2">
         <v>1</v>
       </c>
-      <c r="BG25" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH25" s="2">
+      <c r="BG25" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH25" s="7">
         <v>1</v>
       </c>
       <c r="BI25" s="2">
@@ -6012,7 +6012,7 @@
       <c r="BR25" s="2">
         <v>0</v>
       </c>
-      <c r="BS25" s="2">
+      <c r="BS25" s="1">
         <v>0</v>
       </c>
       <c r="BT25" s="2"/>
@@ -6037,10 +6037,10 @@
       <c r="CE25" s="2">
         <v>1</v>
       </c>
-      <c r="CF25" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG25" s="7">
+      <c r="CF25" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG25" s="2">
         <v>1</v>
       </c>
       <c r="CH25" s="2">
@@ -6172,7 +6172,7 @@
       </c>
     </row>
     <row r="26" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="X26" s="2">
+      <c r="X26" s="7">
         <v>0</v>
       </c>
       <c r="Y26" s="2">
@@ -6205,10 +6205,10 @@
       <c r="AH26" s="2">
         <v>1</v>
       </c>
-      <c r="AI26" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ26" s="2">
+      <c r="AI26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="7">
         <v>1</v>
       </c>
       <c r="AK26" s="2">
@@ -6241,10 +6241,10 @@
       <c r="AT26" s="2">
         <v>1</v>
       </c>
-      <c r="AU26" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV26" s="2">
+      <c r="AU26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV26" s="7">
         <v>1</v>
       </c>
       <c r="AW26" s="2">
@@ -6277,10 +6277,10 @@
       <c r="BF26" s="2">
         <v>1</v>
       </c>
-      <c r="BG26" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH26" s="2">
+      <c r="BG26" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH26" s="7">
         <v>1</v>
       </c>
       <c r="BI26" s="2">
@@ -6313,7 +6313,7 @@
       <c r="BR26" s="2">
         <v>0</v>
       </c>
-      <c r="BS26" s="2">
+      <c r="BS26" s="1">
         <v>0</v>
       </c>
       <c r="BT26" s="2"/>
@@ -6338,10 +6338,10 @@
       <c r="CE26" s="2">
         <v>1</v>
       </c>
-      <c r="CF26" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG26" s="7">
+      <c r="CF26" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG26" s="2">
         <v>1</v>
       </c>
       <c r="CH26" s="2">
@@ -6473,7 +6473,7 @@
       </c>
     </row>
     <row r="27" spans="1:139" x14ac:dyDescent="0.25">
-      <c r="X27" s="2">
+      <c r="X27" s="7">
         <v>0</v>
       </c>
       <c r="Y27" s="2">
@@ -6506,10 +6506,10 @@
       <c r="AH27" s="2">
         <v>1</v>
       </c>
-      <c r="AI27" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ27" s="2">
+      <c r="AI27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ27" s="7">
         <v>1</v>
       </c>
       <c r="AK27" s="2">
@@ -6542,10 +6542,10 @@
       <c r="AT27" s="2">
         <v>1</v>
       </c>
-      <c r="AU27" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV27" s="2">
+      <c r="AU27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV27" s="7">
         <v>1</v>
       </c>
       <c r="AW27" s="2">
@@ -6578,10 +6578,10 @@
       <c r="BF27" s="2">
         <v>1</v>
       </c>
-      <c r="BG27" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH27" s="2">
+      <c r="BG27" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH27" s="7">
         <v>1</v>
       </c>
       <c r="BI27" s="2">
@@ -6614,7 +6614,7 @@
       <c r="BR27" s="2">
         <v>0</v>
       </c>
-      <c r="BS27" s="2">
+      <c r="BS27" s="1">
         <v>0</v>
       </c>
       <c r="BT27" s="2"/>
@@ -6639,10 +6639,10 @@
       <c r="CE27" s="2">
         <v>1</v>
       </c>
-      <c r="CF27" s="1">
-        <v>1</v>
-      </c>
-      <c r="CG27" s="7">
+      <c r="CF27" s="2">
+        <v>1</v>
+      </c>
+      <c r="CG27" s="2">
         <v>1</v>
       </c>
       <c r="CH27" s="2">
@@ -6807,10 +6807,10 @@
       <c r="AH28" s="2">
         <v>1</v>
       </c>
-      <c r="AI28" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ28" s="2">
+      <c r="AI28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="7">
         <v>1</v>
       </c>
       <c r="AK28" s="2">
@@ -6843,10 +6843,10 @@
       <c r="AT28" s="2">
         <v>1</v>
       </c>
-      <c r="AU28" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV28" s="2">
+      <c r="AU28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV28" s="7">
         <v>1</v>
       </c>
       <c r="AW28" s="2">
@@ -6879,10 +6879,10 @@
       <c r="BF28" s="2">
         <v>1</v>
       </c>
-      <c r="BG28" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH28" s="2">
+      <c r="BG28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH28" s="7">
         <v>1</v>
       </c>
       <c r="BI28" s="2">
@@ -6940,10 +6940,10 @@
       <c r="CE28" s="9">
         <v>1</v>
       </c>
-      <c r="CF28" s="10">
-        <v>1</v>
-      </c>
-      <c r="CG28" s="8">
+      <c r="CF28" s="9">
+        <v>1</v>
+      </c>
+      <c r="CG28" s="9">
         <v>1</v>
       </c>
       <c r="CH28" s="9">
@@ -7108,10 +7108,10 @@
       <c r="AH29" s="2">
         <v>1</v>
       </c>
-      <c r="AI29" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ29" s="2">
+      <c r="AI29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="7">
         <v>1</v>
       </c>
       <c r="AK29" s="2">
@@ -7144,10 +7144,10 @@
       <c r="AT29" s="2">
         <v>1</v>
       </c>
-      <c r="AU29" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV29" s="2">
+      <c r="AU29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV29" s="7">
         <v>1</v>
       </c>
       <c r="AW29" s="2">
@@ -7180,10 +7180,10 @@
       <c r="BF29" s="2">
         <v>1</v>
       </c>
-      <c r="BG29" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH29" s="2">
+      <c r="BG29" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH29" s="7">
         <v>1</v>
       </c>
       <c r="BI29" s="2">
@@ -7263,10 +7263,10 @@
       <c r="AH30" s="2">
         <v>1</v>
       </c>
-      <c r="AI30" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ30" s="2">
+      <c r="AI30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="7">
         <v>1</v>
       </c>
       <c r="AK30" s="2">
@@ -7299,10 +7299,10 @@
       <c r="AT30" s="2">
         <v>1</v>
       </c>
-      <c r="AU30" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV30" s="2">
+      <c r="AU30" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV30" s="7">
         <v>1</v>
       </c>
       <c r="AW30" s="2">
@@ -7335,10 +7335,10 @@
       <c r="BF30" s="2">
         <v>1</v>
       </c>
-      <c r="BG30" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH30" s="2">
+      <c r="BG30" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH30" s="7">
         <v>1</v>
       </c>
       <c r="BI30" s="2">
@@ -7418,10 +7418,10 @@
       <c r="AH31" s="2">
         <v>1</v>
       </c>
-      <c r="AI31" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ31" s="2">
+      <c r="AI31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ31" s="7">
         <v>1</v>
       </c>
       <c r="AK31" s="2">
@@ -7454,10 +7454,10 @@
       <c r="AT31" s="2">
         <v>1</v>
       </c>
-      <c r="AU31" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV31" s="2">
+      <c r="AU31" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV31" s="7">
         <v>1</v>
       </c>
       <c r="AW31" s="2">
@@ -7490,10 +7490,10 @@
       <c r="BF31" s="2">
         <v>1</v>
       </c>
-      <c r="BG31" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH31" s="2">
+      <c r="BG31" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH31" s="7">
         <v>1</v>
       </c>
       <c r="BI31" s="2">
@@ -7573,10 +7573,10 @@
       <c r="AH32" s="2">
         <v>1</v>
       </c>
-      <c r="AI32" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ32" s="2">
+      <c r="AI32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ32" s="7">
         <v>1</v>
       </c>
       <c r="AK32" s="2">
@@ -7609,10 +7609,10 @@
       <c r="AT32" s="2">
         <v>1</v>
       </c>
-      <c r="AU32" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV32" s="2">
+      <c r="AU32" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV32" s="7">
         <v>1</v>
       </c>
       <c r="AW32" s="2">
@@ -7645,10 +7645,10 @@
       <c r="BF32" s="2">
         <v>1</v>
       </c>
-      <c r="BG32" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH32" s="2">
+      <c r="BG32" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH32" s="7">
         <v>1</v>
       </c>
       <c r="BI32" s="2">
@@ -7686,294 +7686,294 @@
       </c>
     </row>
     <row r="33" spans="24:71" x14ac:dyDescent="0.25">
-      <c r="X33" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AO33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AP33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AR33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AS33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AT33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AW33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AX33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AY33" s="2">
-        <v>1</v>
-      </c>
-      <c r="AZ33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BA33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BB33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BC33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BD33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BE33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BF33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BG33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BI33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BJ33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BK33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BL33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BN33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BO33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BP33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BQ33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BR33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BS33" s="1">
+      <c r="X33" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="10">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="8">
+        <v>1</v>
+      </c>
+      <c r="AK33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AM33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AN33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AO33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AP33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AQ33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AR33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AS33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AT33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AU33" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV33" s="8">
+        <v>1</v>
+      </c>
+      <c r="AW33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AX33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AY33" s="9">
+        <v>1</v>
+      </c>
+      <c r="AZ33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BA33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BB33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BC33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BD33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BE33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BF33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BG33" s="10">
+        <v>1</v>
+      </c>
+      <c r="BH33" s="8">
+        <v>1</v>
+      </c>
+      <c r="BI33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BJ33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BK33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BN33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BO33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BP33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BR33" s="9">
+        <v>1</v>
+      </c>
+      <c r="BS33" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="24:71" x14ac:dyDescent="0.25">
-      <c r="X34" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y34" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AK34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AL34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AM34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AN34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AO34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AP34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AQ34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AR34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AS34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AT34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AU34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AV34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AW34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AX34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AY34" s="2">
-        <v>1</v>
-      </c>
-      <c r="AZ34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BA34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BB34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BC34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BD34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BE34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BF34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BG34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BI34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BJ34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BK34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BL34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BN34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BO34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BP34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BQ34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BR34" s="2">
-        <v>1</v>
-      </c>
-      <c r="BS34" s="1">
+      <c r="X34" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI34" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AK34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AL34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AM34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AN34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AO34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AP34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AQ34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AR34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AS34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AT34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AU34" s="6">
+        <v>1</v>
+      </c>
+      <c r="AV34" s="4">
+        <v>1</v>
+      </c>
+      <c r="AW34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AX34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AY34" s="5">
+        <v>1</v>
+      </c>
+      <c r="AZ34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BA34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BB34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BC34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BD34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BE34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BF34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BG34" s="6">
+        <v>1</v>
+      </c>
+      <c r="BH34" s="4">
+        <v>1</v>
+      </c>
+      <c r="BI34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BJ34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BK34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BL34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BM34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BN34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BO34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BP34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BQ34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BR34" s="5">
+        <v>1</v>
+      </c>
+      <c r="BS34" s="6">
         <v>1</v>
       </c>
     </row>
@@ -8011,10 +8011,10 @@
       <c r="AH35" s="2">
         <v>1</v>
       </c>
-      <c r="AI35" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ35" s="2">
+      <c r="AI35" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ35" s="7">
         <v>1</v>
       </c>
       <c r="AK35" s="2">
@@ -8047,10 +8047,10 @@
       <c r="AT35" s="9">
         <v>1</v>
       </c>
-      <c r="AU35" s="9">
-        <v>1</v>
-      </c>
-      <c r="AV35" s="9">
+      <c r="AU35" s="10">
+        <v>1</v>
+      </c>
+      <c r="AV35" s="8">
         <v>1</v>
       </c>
       <c r="AW35" s="9">
@@ -8083,10 +8083,10 @@
       <c r="BF35" s="2">
         <v>1</v>
       </c>
-      <c r="BG35" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH35" s="2">
+      <c r="BG35" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH35" s="7">
         <v>1</v>
       </c>
       <c r="BI35" s="2">
@@ -8157,10 +8157,10 @@
       <c r="AH36" s="2">
         <v>1</v>
       </c>
-      <c r="AI36" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ36" s="2">
+      <c r="AI36" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="7">
         <v>1</v>
       </c>
       <c r="AK36" s="2">
@@ -8193,10 +8193,10 @@
       <c r="AT36" s="2">
         <v>0</v>
       </c>
-      <c r="AU36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV36" s="2">
+      <c r="AU36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV36" s="7">
         <v>0</v>
       </c>
       <c r="AW36" s="2">
@@ -8229,10 +8229,10 @@
       <c r="BF36" s="2">
         <v>1</v>
       </c>
-      <c r="BG36" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH36" s="2">
+      <c r="BG36" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH36" s="7">
         <v>1</v>
       </c>
       <c r="BI36" s="2">
@@ -8303,10 +8303,10 @@
       <c r="AH37" s="2">
         <v>1</v>
       </c>
-      <c r="AI37" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ37" s="2">
+      <c r="AI37" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ37" s="7">
         <v>1</v>
       </c>
       <c r="AK37" s="2">
@@ -8339,10 +8339,10 @@
       <c r="AT37" s="2">
         <v>0</v>
       </c>
-      <c r="AU37" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV37" s="2">
+      <c r="AU37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV37" s="7">
         <v>0</v>
       </c>
       <c r="AW37" s="2">
@@ -8375,10 +8375,10 @@
       <c r="BF37" s="2">
         <v>1</v>
       </c>
-      <c r="BG37" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH37" s="2">
+      <c r="BG37" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH37" s="7">
         <v>1</v>
       </c>
       <c r="BI37" s="2">
@@ -8449,10 +8449,10 @@
       <c r="AH38" s="2">
         <v>1</v>
       </c>
-      <c r="AI38" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ38" s="2">
+      <c r="AI38" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ38" s="7">
         <v>1</v>
       </c>
       <c r="AK38" s="2">
@@ -8485,10 +8485,10 @@
       <c r="AT38" s="2">
         <v>0</v>
       </c>
-      <c r="AU38" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV38" s="2">
+      <c r="AU38" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV38" s="7">
         <v>0</v>
       </c>
       <c r="AW38" s="2">
@@ -8521,10 +8521,10 @@
       <c r="BF38" s="2">
         <v>1</v>
       </c>
-      <c r="BG38" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH38" s="2">
+      <c r="BG38" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH38" s="7">
         <v>1</v>
       </c>
       <c r="BI38" s="2">
@@ -8595,10 +8595,10 @@
       <c r="AH39" s="2">
         <v>1</v>
       </c>
-      <c r="AI39" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ39" s="2">
+      <c r="AI39" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="7">
         <v>1</v>
       </c>
       <c r="AK39" s="2">
@@ -8631,10 +8631,10 @@
       <c r="AT39" s="2">
         <v>0</v>
       </c>
-      <c r="AU39" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV39" s="2">
+      <c r="AU39" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV39" s="7">
         <v>0</v>
       </c>
       <c r="AW39" s="2">
@@ -8667,10 +8667,10 @@
       <c r="BF39" s="2">
         <v>1</v>
       </c>
-      <c r="BG39" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH39" s="2">
+      <c r="BG39" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH39" s="7">
         <v>1</v>
       </c>
       <c r="BI39" s="2">
@@ -8741,10 +8741,10 @@
       <c r="AH40" s="2">
         <v>1</v>
       </c>
-      <c r="AI40" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ40" s="2">
+      <c r="AI40" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="7">
         <v>1</v>
       </c>
       <c r="AK40" s="2">
@@ -8777,10 +8777,10 @@
       <c r="AT40" s="2">
         <v>0</v>
       </c>
-      <c r="AU40" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV40" s="2">
+      <c r="AU40" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV40" s="7">
         <v>0</v>
       </c>
       <c r="AW40" s="2">
@@ -8813,10 +8813,10 @@
       <c r="BF40" s="2">
         <v>1</v>
       </c>
-      <c r="BG40" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH40" s="2">
+      <c r="BG40" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH40" s="7">
         <v>1</v>
       </c>
       <c r="BI40" s="2">
@@ -8887,10 +8887,10 @@
       <c r="AH41" s="2">
         <v>1</v>
       </c>
-      <c r="AI41" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ41" s="2">
+      <c r="AI41" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ41" s="7">
         <v>1</v>
       </c>
       <c r="AK41" s="2">
@@ -8923,10 +8923,10 @@
       <c r="AT41" s="2">
         <v>0</v>
       </c>
-      <c r="AU41" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV41" s="2">
+      <c r="AU41" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV41" s="7">
         <v>0</v>
       </c>
       <c r="AW41" s="2">
@@ -8959,10 +8959,10 @@
       <c r="BF41" s="2">
         <v>1</v>
       </c>
-      <c r="BG41" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH41" s="2">
+      <c r="BG41" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH41" s="7">
         <v>1</v>
       </c>
       <c r="BI41" s="2">
@@ -9033,10 +9033,10 @@
       <c r="AH42" s="2">
         <v>1</v>
       </c>
-      <c r="AI42" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ42" s="2">
+      <c r="AI42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ42" s="7">
         <v>1</v>
       </c>
       <c r="AK42" s="1">
@@ -9069,10 +9069,10 @@
       <c r="AT42" s="2">
         <v>0</v>
       </c>
-      <c r="AU42" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV42" s="2">
+      <c r="AU42" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV42" s="7">
         <v>0</v>
       </c>
       <c r="AW42" s="2">
@@ -9105,10 +9105,10 @@
       <c r="BF42" s="7">
         <v>1</v>
       </c>
-      <c r="BG42" s="2">
-        <v>1</v>
-      </c>
-      <c r="BH42" s="2">
+      <c r="BG42" s="1">
+        <v>1</v>
+      </c>
+      <c r="BH42" s="7">
         <v>1</v>
       </c>
       <c r="BI42" s="2">
@@ -9179,10 +9179,10 @@
       <c r="AH43" s="2">
         <v>1</v>
       </c>
-      <c r="AI43" s="2">
-        <v>1</v>
-      </c>
-      <c r="AJ43" s="9">
+      <c r="AI43" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ43" s="8">
         <v>1</v>
       </c>
       <c r="AK43" s="10">
@@ -9215,10 +9215,10 @@
       <c r="AT43" s="2">
         <v>0</v>
       </c>
-      <c r="AU43" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV43" s="2">
+      <c r="AU43" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV43" s="7">
         <v>0</v>
       </c>
       <c r="AW43" s="2">
@@ -9251,10 +9251,10 @@
       <c r="BF43" s="8">
         <v>1</v>
       </c>
-      <c r="BG43" s="9">
-        <v>1</v>
-      </c>
-      <c r="BH43" s="2">
+      <c r="BG43" s="10">
+        <v>1</v>
+      </c>
+      <c r="BH43" s="7">
         <v>1</v>
       </c>
       <c r="BI43" s="2">
@@ -9328,7 +9328,7 @@
       <c r="AI44" s="1">
         <v>1</v>
       </c>
-      <c r="AJ44" s="2">
+      <c r="AJ44" s="7">
         <v>0</v>
       </c>
       <c r="AK44" s="2">
@@ -9361,10 +9361,10 @@
       <c r="AT44" s="2">
         <v>0</v>
       </c>
-      <c r="AU44" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV44" s="2">
+      <c r="AU44" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV44" s="7">
         <v>0</v>
       </c>
       <c r="AW44" s="2">
@@ -9397,7 +9397,7 @@
       <c r="BF44" s="2">
         <v>0</v>
       </c>
-      <c r="BG44" s="2">
+      <c r="BG44" s="1">
         <v>0</v>
       </c>
       <c r="BH44" s="7">
@@ -9438,148 +9438,148 @@
       </c>
     </row>
     <row r="45" spans="24:71" x14ac:dyDescent="0.25">
-      <c r="X45" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y45" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AD45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AE45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AF45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AH45" s="2">
-        <v>1</v>
-      </c>
-      <c r="AI45" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BD45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BE45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BG45" s="2">
-        <v>0</v>
-      </c>
-      <c r="BH45" s="7">
-        <v>1</v>
-      </c>
-      <c r="BI45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BJ45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BK45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BL45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BM45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BN45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BO45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BP45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BQ45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BR45" s="2">
-        <v>1</v>
-      </c>
-      <c r="BS45" s="1">
+      <c r="X45" s="8">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH45" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI45" s="10">
+        <v>1</v>
+      </c>
+      <c r="AJ45" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AQ45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AT45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AU45" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV45" s="8">
+        <v>0</v>
+      </c>
+      <c r="AW45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AX45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AY45" s="9">
+        <v>0</v>
+      </c>
+      <c r="AZ45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BA45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BB45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BC45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BD45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BE45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BF45" s="9">
+        <v>0</v>
+      </c>
+      <c r="BG45" s="10">
+        <v>0</v>
+      </c>
+      <c r="BH45" s="8">
+        <v>1</v>
+      </c>
+      <c r="BI45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BJ45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BK45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BL45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BM45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BN45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BO45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BP45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BQ45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BR45" s="9">
+        <v>1</v>
+      </c>
+      <c r="BS45" s="10">
         <v>1</v>
       </c>
     </row>
@@ -9620,76 +9620,76 @@
       <c r="AI46" s="1">
         <v>1</v>
       </c>
-      <c r="AJ46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BD46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BE46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF46" s="2">
-        <v>0</v>
-      </c>
-      <c r="BG46" s="2">
+      <c r="AJ46" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AN46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AO46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AP46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AQ46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AR46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AS46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AT46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AU46" s="6">
+        <v>0</v>
+      </c>
+      <c r="AV46" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AX46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AY46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AZ46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BA46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BB46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BC46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BD46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BE46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BF46" s="5">
+        <v>0</v>
+      </c>
+      <c r="BG46" s="6">
         <v>0</v>
       </c>
       <c r="BH46" s="7">
@@ -9766,7 +9766,7 @@
       <c r="AI47" s="1">
         <v>1</v>
       </c>
-      <c r="AJ47" s="2">
+      <c r="AJ47" s="7">
         <v>0</v>
       </c>
       <c r="AK47" s="2">
@@ -9799,10 +9799,10 @@
       <c r="AT47" s="2">
         <v>0</v>
       </c>
-      <c r="AU47" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV47" s="2">
+      <c r="AU47" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV47" s="7">
         <v>0</v>
       </c>
       <c r="AW47" s="2">
@@ -9835,7 +9835,7 @@
       <c r="BF47" s="2">
         <v>0</v>
       </c>
-      <c r="BG47" s="2">
+      <c r="BG47" s="1">
         <v>0</v>
       </c>
       <c r="BH47" s="7">
@@ -9912,7 +9912,7 @@
       <c r="AI48" s="1">
         <v>1</v>
       </c>
-      <c r="AJ48" s="2">
+      <c r="AJ48" s="7">
         <v>0</v>
       </c>
       <c r="AK48" s="2">
@@ -9945,10 +9945,10 @@
       <c r="AT48" s="2">
         <v>0</v>
       </c>
-      <c r="AU48" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV48" s="2">
+      <c r="AU48" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV48" s="7">
         <v>0</v>
       </c>
       <c r="AW48" s="2">
@@ -9981,7 +9981,7 @@
       <c r="BF48" s="2">
         <v>0</v>
       </c>
-      <c r="BG48" s="2">
+      <c r="BG48" s="1">
         <v>0</v>
       </c>
       <c r="BH48" s="7">
@@ -10058,7 +10058,7 @@
       <c r="AI49" s="1">
         <v>1</v>
       </c>
-      <c r="AJ49" s="2">
+      <c r="AJ49" s="7">
         <v>0</v>
       </c>
       <c r="AK49" s="2">
@@ -10091,10 +10091,10 @@
       <c r="AT49" s="2">
         <v>0</v>
       </c>
-      <c r="AU49" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV49" s="2">
+      <c r="AU49" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV49" s="7">
         <v>0</v>
       </c>
       <c r="AW49" s="2">
@@ -10127,7 +10127,7 @@
       <c r="BF49" s="2">
         <v>0</v>
       </c>
-      <c r="BG49" s="2">
+      <c r="BG49" s="1">
         <v>0</v>
       </c>
       <c r="BH49" s="7">
@@ -10204,7 +10204,7 @@
       <c r="AI50" s="1">
         <v>1</v>
       </c>
-      <c r="AJ50" s="2">
+      <c r="AJ50" s="7">
         <v>0</v>
       </c>
       <c r="AK50" s="2">
@@ -10237,10 +10237,10 @@
       <c r="AT50" s="2">
         <v>0</v>
       </c>
-      <c r="AU50" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV50" s="2">
+      <c r="AU50" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV50" s="7">
         <v>0</v>
       </c>
       <c r="AW50" s="2">
@@ -10273,7 +10273,7 @@
       <c r="BF50" s="2">
         <v>0</v>
       </c>
-      <c r="BG50" s="2">
+      <c r="BG50" s="1">
         <v>0</v>
       </c>
       <c r="BH50" s="7">
@@ -10350,7 +10350,7 @@
       <c r="AI51" s="1">
         <v>1</v>
       </c>
-      <c r="AJ51" s="2">
+      <c r="AJ51" s="7">
         <v>0</v>
       </c>
       <c r="AK51" s="2">
@@ -10383,10 +10383,10 @@
       <c r="AT51" s="2">
         <v>0</v>
       </c>
-      <c r="AU51" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV51" s="2">
+      <c r="AU51" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV51" s="7">
         <v>0</v>
       </c>
       <c r="AW51" s="2">
@@ -10419,7 +10419,7 @@
       <c r="BF51" s="2">
         <v>0</v>
       </c>
-      <c r="BG51" s="2">
+      <c r="BG51" s="1">
         <v>0</v>
       </c>
       <c r="BH51" s="7">
@@ -10496,7 +10496,7 @@
       <c r="AI52" s="1">
         <v>1</v>
       </c>
-      <c r="AJ52" s="2">
+      <c r="AJ52" s="7">
         <v>0</v>
       </c>
       <c r="AK52" s="2">
@@ -10529,10 +10529,10 @@
       <c r="AT52" s="2">
         <v>0</v>
       </c>
-      <c r="AU52" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV52" s="2">
+      <c r="AU52" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV52" s="7">
         <v>0</v>
       </c>
       <c r="AW52" s="2">
@@ -10565,7 +10565,7 @@
       <c r="BF52" s="2">
         <v>0</v>
       </c>
-      <c r="BG52" s="2">
+      <c r="BG52" s="1">
         <v>0</v>
       </c>
       <c r="BH52" s="7">
@@ -10642,7 +10642,7 @@
       <c r="AI53" s="1">
         <v>1</v>
       </c>
-      <c r="AJ53" s="2">
+      <c r="AJ53" s="7">
         <v>0</v>
       </c>
       <c r="AK53" s="2">
@@ -10675,10 +10675,10 @@
       <c r="AT53" s="2">
         <v>0</v>
       </c>
-      <c r="AU53" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV53" s="2">
+      <c r="AU53" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV53" s="7">
         <v>0</v>
       </c>
       <c r="AW53" s="2">
@@ -10711,7 +10711,7 @@
       <c r="BF53" s="2">
         <v>0</v>
       </c>
-      <c r="BG53" s="2">
+      <c r="BG53" s="1">
         <v>0</v>
       </c>
       <c r="BH53" s="7">
@@ -10788,7 +10788,7 @@
       <c r="AI54" s="1">
         <v>1</v>
       </c>
-      <c r="AJ54" s="2">
+      <c r="AJ54" s="7">
         <v>0</v>
       </c>
       <c r="AK54" s="2">
@@ -10821,10 +10821,10 @@
       <c r="AT54" s="2">
         <v>0</v>
       </c>
-      <c r="AU54" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV54" s="2">
+      <c r="AU54" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV54" s="7">
         <v>0</v>
       </c>
       <c r="AW54" s="2">
@@ -10857,7 +10857,7 @@
       <c r="BF54" s="2">
         <v>0</v>
       </c>
-      <c r="BG54" s="2">
+      <c r="BG54" s="1">
         <v>0</v>
       </c>
       <c r="BH54" s="7">
@@ -10934,7 +10934,7 @@
       <c r="AI55" s="1">
         <v>1</v>
       </c>
-      <c r="AJ55" s="2">
+      <c r="AJ55" s="7">
         <v>0</v>
       </c>
       <c r="AK55" s="2">
@@ -10967,10 +10967,10 @@
       <c r="AT55" s="2">
         <v>0</v>
       </c>
-      <c r="AU55" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV55" s="2">
+      <c r="AU55" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV55" s="7">
         <v>0</v>
       </c>
       <c r="AW55" s="2">
@@ -11003,7 +11003,7 @@
       <c r="BF55" s="2">
         <v>0</v>
       </c>
-      <c r="BG55" s="2">
+      <c r="BG55" s="1">
         <v>0</v>
       </c>
       <c r="BH55" s="7">
@@ -11080,7 +11080,7 @@
       <c r="AI56" s="1">
         <v>1</v>
       </c>
-      <c r="AJ56" s="2">
+      <c r="AJ56" s="7">
         <v>0</v>
       </c>
       <c r="AK56" s="2">
@@ -11113,10 +11113,10 @@
       <c r="AT56" s="2">
         <v>0</v>
       </c>
-      <c r="AU56" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV56" s="2">
+      <c r="AU56" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV56" s="7">
         <v>0</v>
       </c>
       <c r="AW56" s="2">
@@ -11149,7 +11149,7 @@
       <c r="BF56" s="2">
         <v>0</v>
       </c>
-      <c r="BG56" s="2">
+      <c r="BG56" s="1">
         <v>0</v>
       </c>
       <c r="BH56" s="7">
@@ -11226,76 +11226,76 @@
       <c r="AI57" s="10">
         <v>1</v>
       </c>
-      <c r="AJ57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AP57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AQ57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AR57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AS57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AT57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AU57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AV57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AW57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AX57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AY57" s="2">
-        <v>0</v>
-      </c>
-      <c r="AZ57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BA57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BB57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BC57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BD57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BE57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF57" s="2">
-        <v>0</v>
-      </c>
-      <c r="BG57" s="2">
+      <c r="AJ57" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AM57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AN57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AO57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AP57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AQ57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AR57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AS57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AT57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AU57" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV57" s="8">
+        <v>0</v>
+      </c>
+      <c r="AW57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AX57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AY57" s="9">
+        <v>0</v>
+      </c>
+      <c r="AZ57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BA57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BB57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BC57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BD57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BE57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BF57" s="9">
+        <v>0</v>
+      </c>
+      <c r="BG57" s="10">
         <v>0</v>
       </c>
       <c r="BH57" s="8">

</xml_diff>